<commit_message>
feat: 🎸 continuos chatbot answer question
</commit_message>
<xml_diff>
--- a/chatbot/csv/Hatyai_restaurant.xlsx
+++ b/chatbot/csv/Hatyai_restaurant.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Laantachou</t>
   </si>
   <si>
-    <t xml:space="preserve">Steak, A la carte</t>
+    <t xml:space="preserve">Steak,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">No</t>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Longhua malatang</t>
   </si>
   <si>
-    <t xml:space="preserve">Shabu, Sukiyaki, Hotpot, Buffet</t>
+    <t xml:space="preserve">Shabu,Sukiyaki,Hotpot,Buffet</t>
   </si>
   <si>
     <t xml:space="preserve">฿</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Blackbridge Halal Steakhouse &amp; Restaurant</t>
   </si>
   <si>
-    <t xml:space="preserve">Halal, Burger, Steak</t>
+    <t xml:space="preserve">Halal,Burger,Steak</t>
   </si>
   <si>
     <t xml:space="preserve">฿฿฿</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Meats And Beans</t>
   </si>
   <si>
-    <t xml:space="preserve">American, Steak, Grill</t>
+    <t xml:space="preserve">American,Steak,Grill</t>
   </si>
   <si>
     <t xml:space="preserve">Wednesday</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Chokdeebuttim Bah Kut Teh Hatyai</t>
   </si>
   <si>
-    <t xml:space="preserve">Dim sum, Chinese</t>
+    <t xml:space="preserve">Dimsum,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">0805259623</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Lunyin ก๋วยจั๊บหมูกรอบ</t>
   </si>
   <si>
-    <t xml:space="preserve">Pork belly, Noodles</t>
+    <t xml:space="preserve">Porkbelly,Noodles</t>
   </si>
   <si>
     <t xml:space="preserve">Sunday</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">Go-Oun</t>
   </si>
   <si>
-    <t xml:space="preserve">Chinese, Dim sum</t>
+    <t xml:space="preserve">Chinese,Dimsum</t>
   </si>
   <si>
     <t xml:space="preserve">Tuesday</t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">Nai Roo</t>
   </si>
   <si>
-    <t xml:space="preserve">A la carte, Chinese</t>
+    <t xml:space="preserve">Alacarte,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">074237680</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">Baan Krua</t>
   </si>
   <si>
-    <t xml:space="preserve">Cafe, Coffee, Tea, Thai</t>
+    <t xml:space="preserve">Cafe,Coffee,Tea,Thai</t>
   </si>
   <si>
     <t xml:space="preserve">0637304619</t>
@@ -227,7 +227,7 @@
     <t xml:space="preserve">Daa Yihng Betong</t>
   </si>
   <si>
-    <t xml:space="preserve">Chinese, A la carte</t>
+    <t xml:space="preserve">Chinese,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">074354051</t>
@@ -269,7 +269,7 @@
     <t xml:space="preserve">Imhouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Cafe, Coffee, Tea, Bakery, Cake</t>
+    <t xml:space="preserve">Cafe,Coffee,Tea,Bakery,Cake</t>
   </si>
   <si>
     <t xml:space="preserve">0835944281</t>
@@ -281,7 +281,7 @@
     <t xml:space="preserve">Moo Tod Mister Tum Tum Thung Sao</t>
   </si>
   <si>
-    <t xml:space="preserve">Street food</t>
+    <t xml:space="preserve">Streetfood</t>
   </si>
   <si>
     <t xml:space="preserve">0810807010</t>
@@ -293,7 +293,7 @@
     <t xml:space="preserve">Kway Teow End Duangthoon</t>
   </si>
   <si>
-    <t xml:space="preserve">Noodles, A la carte, Chinese</t>
+    <t xml:space="preserve">Noodles,Alacarte,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">Thursday</t>
@@ -305,7 +305,7 @@
     <t xml:space="preserve">Sushi Champion</t>
   </si>
   <si>
-    <t xml:space="preserve">Japanese, Sushi</t>
+    <t xml:space="preserve">Japanese,Sushi</t>
   </si>
   <si>
     <t xml:space="preserve">0973450868</t>
@@ -326,7 +326,7 @@
     <t xml:space="preserve">Som Tum Hua Pan</t>
   </si>
   <si>
-    <t xml:space="preserve">Thai Northeastern, Som Tum</t>
+    <t xml:space="preserve">ThaiNortheastern,SomTum</t>
   </si>
   <si>
     <t xml:space="preserve">0895963272</t>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">CLAY</t>
   </si>
   <si>
-    <t xml:space="preserve">Cafe, Italian, American</t>
+    <t xml:space="preserve">Cafe,Italian,American</t>
   </si>
   <si>
     <t xml:space="preserve">0828279154</t>
@@ -350,7 +350,7 @@
     <t xml:space="preserve">Prik Khi Nu Mu Kratha</t>
   </si>
   <si>
-    <t xml:space="preserve">Mu Kratha, Buffet</t>
+    <t xml:space="preserve">MuKratha,Buffet</t>
   </si>
   <si>
     <t xml:space="preserve">098589864</t>
@@ -362,7 +362,7 @@
     <t xml:space="preserve">The Basil</t>
   </si>
   <si>
-    <t xml:space="preserve">Italian, Steak</t>
+    <t xml:space="preserve">Italian,Steak</t>
   </si>
   <si>
     <t xml:space="preserve">0818919321</t>
@@ -383,7 +383,7 @@
     <t xml:space="preserve">Humble Farm Kitchen</t>
   </si>
   <si>
-    <t xml:space="preserve">Healthy, Salad, Cafe, Fusion</t>
+    <t xml:space="preserve">Healthy,Salad,Cafe,Fusion</t>
   </si>
   <si>
     <t xml:space="preserve">0622429844</t>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">Moo Boran</t>
   </si>
   <si>
-    <t xml:space="preserve">Thai, A la carte</t>
+    <t xml:space="preserve">Thai,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">0869615738</t>
@@ -407,7 +407,7 @@
     <t xml:space="preserve">Lorem Ipsum space</t>
   </si>
   <si>
-    <t xml:space="preserve">Cafe, Coffee, Tea</t>
+    <t xml:space="preserve">Cafe,Coffee,Tea</t>
   </si>
   <si>
     <t xml:space="preserve">0635263554</t>
@@ -428,7 +428,7 @@
     <t xml:space="preserve">Yiean Sukiyaki Hotpot Chinese</t>
   </si>
   <si>
-    <t xml:space="preserve">Shabu, Sukiyaki, Hotpot, Buffet, Chinese</t>
+    <t xml:space="preserve">Shabu,Sukiyaki,Hotpot,Buffet,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">0648517688</t>
@@ -440,7 +440,7 @@
     <t xml:space="preserve">Monmsomsod</t>
   </si>
   <si>
-    <t xml:space="preserve">Thai, A la carte, Coffee, Tea</t>
+    <t xml:space="preserve">Thai,Alacarte,Coffee,Tea</t>
   </si>
   <si>
     <t xml:space="preserve">0842299288</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">Grommee Kai</t>
   </si>
   <si>
-    <t xml:space="preserve">Noodles, Fried noodles</t>
+    <t xml:space="preserve">Noodles,Friednoodles</t>
   </si>
   <si>
     <t xml:space="preserve">074232150</t>
@@ -476,7 +476,7 @@
     <t xml:space="preserve">Yamaumi Ramen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ramen, Japanese</t>
+    <t xml:space="preserve">Ramen,Japanese</t>
   </si>
   <si>
     <t xml:space="preserve">0964654496</t>
@@ -497,7 +497,7 @@
     <t xml:space="preserve">Shabushi</t>
   </si>
   <si>
-    <t xml:space="preserve">Shabu, Sukiyaki, Hotpot, Buffet, Japanese</t>
+    <t xml:space="preserve">Shabu,Sukiyaki,Hotpot,Buffet,Japanese</t>
   </si>
   <si>
     <t xml:space="preserve">0952074706</t>
@@ -542,7 +542,7 @@
     <t xml:space="preserve">I AM SALAD</t>
   </si>
   <si>
-    <t xml:space="preserve">Healthy, Salad, Cafe, A la carte, Coffee, Tea</t>
+    <t xml:space="preserve">Healthy,Salad,Cafe,Alacarte,Coffee,Tea</t>
   </si>
   <si>
     <t xml:space="preserve">0919489109</t>
@@ -554,7 +554,7 @@
     <t xml:space="preserve">The Salad</t>
   </si>
   <si>
-    <t xml:space="preserve">Healthy, Salad</t>
+    <t xml:space="preserve">Healthy,Salad</t>
   </si>
   <si>
     <t xml:space="preserve">0816908770</t>
@@ -575,7 +575,7 @@
     <t xml:space="preserve">Ootoya</t>
   </si>
   <si>
-    <t xml:space="preserve">Japanese, A la carte</t>
+    <t xml:space="preserve">Japanese,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">0922494724</t>
@@ -599,7 +599,7 @@
     <t xml:space="preserve">Kanomjeen PaChuen</t>
   </si>
   <si>
-    <t xml:space="preserve">Thai, Dessert</t>
+    <t xml:space="preserve">Thai,Dessert</t>
   </si>
   <si>
     <t xml:space="preserve">0869556117</t>
@@ -614,7 +614,7 @@
     <t xml:space="preserve">Pa Yang</t>
   </si>
   <si>
-    <t xml:space="preserve">Thai, Chinese</t>
+    <t xml:space="preserve">Thai,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">074300556</t>
@@ -626,7 +626,7 @@
     <t xml:space="preserve">Have a bread day</t>
   </si>
   <si>
-    <t xml:space="preserve">Dessert, Cake, Bakery, Cafe, Coffee, Tea</t>
+    <t xml:space="preserve">Dessert,Cake,Bakery,Cafe,Coffee,Tea</t>
   </si>
   <si>
     <t xml:space="preserve">0973453050</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">Kao Tom Rod Dang</t>
   </si>
   <si>
-    <t xml:space="preserve">Street food, A la carte</t>
+    <t xml:space="preserve">Streetfood,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">0897397047</t>
@@ -707,7 +707,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Japanese, Sushi, Buffet</t>
+    <t xml:space="preserve">Japanese,Sushi,Buffet</t>
   </si>
   <si>
     <t xml:space="preserve">074803348</t>
@@ -731,7 +731,7 @@
     <t xml:space="preserve">BonChon</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast food, Korean</t>
+    <t xml:space="preserve">Fastfood,Korean</t>
   </si>
   <si>
     <t xml:space="preserve">0659506845</t>
@@ -770,7 +770,7 @@
     <t xml:space="preserve">Pappardelle</t>
   </si>
   <si>
-    <t xml:space="preserve">Salad, Healthy</t>
+    <t xml:space="preserve">Salad,Healthy</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.google.com/maps/search/?api=1&amp;query=7.0012130999999815,100.47047940000009</t>
@@ -779,7 +779,7 @@
     <t xml:space="preserve">Starbucks</t>
   </si>
   <si>
-    <t xml:space="preserve">Coffee, Tea, Dessert, Cafe</t>
+    <t xml:space="preserve">Coffee,Tea,Dessert,Cafe</t>
   </si>
   <si>
     <t xml:space="preserve">0922798164</t>
@@ -791,7 +791,7 @@
     <t xml:space="preserve">MAKE YOU MINE</t>
   </si>
   <si>
-    <t xml:space="preserve">Dessert, Cake, Bakery, Cafe, Coffee, Tea, Breakfast</t>
+    <t xml:space="preserve">Dessert,Cake,Bakery,Cafe,Coffee,Tea,Breakfast</t>
   </si>
   <si>
     <t xml:space="preserve">0645401444</t>
@@ -833,7 +833,7 @@
     <t xml:space="preserve">Mongmoon Rooftop Bar &amp; Bistro</t>
   </si>
   <si>
-    <t xml:space="preserve">Bar, Fusion, Italian</t>
+    <t xml:space="preserve">Bar,Fusion,Italian</t>
   </si>
   <si>
     <t xml:space="preserve">0621064025</t>
@@ -845,7 +845,7 @@
     <t xml:space="preserve">Lunaray</t>
   </si>
   <si>
-    <t xml:space="preserve">Cafe, Dessert</t>
+    <t xml:space="preserve">Cafe,Dessert</t>
   </si>
   <si>
     <t xml:space="preserve">0831857661</t>
@@ -866,7 +866,7 @@
     <t xml:space="preserve">Kindergarden Hat Yai</t>
   </si>
   <si>
-    <t xml:space="preserve">Fusion, A la carte</t>
+    <t xml:space="preserve">Fusion,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">0973615056</t>
@@ -878,7 +878,7 @@
     <t xml:space="preserve">Homie</t>
   </si>
   <si>
-    <t xml:space="preserve">Ice cream, Cafe, Dessert</t>
+    <t xml:space="preserve">Icecream,Cafe,Dessert</t>
   </si>
   <si>
     <t xml:space="preserve">0641956467</t>
@@ -890,7 +890,7 @@
     <t xml:space="preserve">Arleang Mala</t>
   </si>
   <si>
-    <t xml:space="preserve">Grill, Noodles, Fried noodles, Chinese</t>
+    <t xml:space="preserve">Grill,Noodles,Friednoodles,Chinese</t>
   </si>
   <si>
     <t xml:space="preserve">0828298038</t>
@@ -911,7 +911,7 @@
     <t xml:space="preserve">BAROFFEE CAFÉ</t>
   </si>
   <si>
-    <t xml:space="preserve">Tea, Coffee, Breakfast</t>
+    <t xml:space="preserve">Tea,Coffee,Breakfast</t>
   </si>
   <si>
     <t xml:space="preserve">0843435129</t>
@@ -932,7 +932,7 @@
     <t xml:space="preserve">Burg Republic</t>
   </si>
   <si>
-    <t xml:space="preserve">Burger, Fast food, Halal</t>
+    <t xml:space="preserve">Burger,Fastfood,Halal</t>
   </si>
   <si>
     <t xml:space="preserve">0621818855</t>
@@ -962,7 +962,7 @@
     <t xml:space="preserve">SAENG THONG PHOCHANA</t>
   </si>
   <si>
-    <t xml:space="preserve">Seafood, A la carte</t>
+    <t xml:space="preserve">Seafood,Alacarte</t>
   </si>
   <si>
     <t xml:space="preserve">074580789</t>
@@ -980,7 +980,7 @@
     <t xml:space="preserve">Hasul Korean Cafe And Restaurant</t>
   </si>
   <si>
-    <t xml:space="preserve">Korean, Fusiom, Dessert</t>
+    <t xml:space="preserve">Korean,Fusiom,Dessert</t>
   </si>
   <si>
     <t xml:space="preserve">0902095301</t>
@@ -1256,7 +1256,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="28.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: 🎸 choose time period
</commit_message>
<xml_diff>
--- a/chatbot/csv/Hatyai_restaurant.xlsx
+++ b/chatbot/csv/Hatyai_restaurant.xlsx
@@ -980,7 +980,7 @@
     <t xml:space="preserve">Hasul Korean Cafe And Restaurant</t>
   </si>
   <si>
-    <t xml:space="preserve">Korean,Fusiom,Dessert</t>
+    <t xml:space="preserve">Korean,Fusion,Dessert</t>
   </si>
   <si>
     <t xml:space="preserve">0902095301</t>
@@ -1255,8 +1255,8 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B80" activeCellId="0" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="28.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>